<commit_message>
Modelos Mesa e Ingreso unidos a la logica de los views
</commit_message>
<xml_diff>
--- a/static/InvitadosEvento.xlsx
+++ b/static/InvitadosEvento.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
@@ -469,7 +469,11 @@
           <t>Numero</t>
         </is>
       </c>
-      <c r="C1" s="2" t="n"/>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Mesa</t>
+        </is>
+      </c>
       <c r="D1" s="2" t="n"/>
       <c r="E1" s="2" t="n"/>
       <c r="F1" s="2" t="n"/>
@@ -489,36 +493,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Paolo Cetti</t>
+          <t>Mouse</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5493516450124</t>
-        </is>
+          <t>+549456</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>Paolo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>test</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Paolo Cetti</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>+5493516450124</t>
+          <t>+549</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change Mesa y extend de djangosite
</commit_message>
<xml_diff>
--- a/static/InvitadosEvento.xlsx
+++ b/static/InvitadosEvento.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
@@ -493,33 +493,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mouse</t>
+          <t>Paolo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+549456</t>
+          <t>+549</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Paolo</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>+549</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>